<commit_message>
update ner, logreg, tingkat keparahan
</commit_message>
<xml_diff>
--- a/QE Statistik V2/hasilQE_new/QE_Stat_V2_testing_result_what.xlsx
+++ b/QE Statistik V2/hasilQE_new/QE_Stat_V2_testing_result_what.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adi/Desktop/TA_Adi_V2/QE Statistik V2/hasilQE_new/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64963137-641B-F04E-AAA7-1D7D068E08A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB35B484-3106-FA40-A268-6943C983C969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1650,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G91" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G128" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>

</xml_diff>